<commit_message>
Add file open check and reset study buttons functionality; enhance Studying timer logic
</commit_message>
<xml_diff>
--- a/store/analytics.xlsx
+++ b/store/analytics.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,10 +469,26 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>45688.85437041675</v>
+        <v>45688.88619232639</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>45688.85441850901</v>
+        <v>45688.88624818287</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>MAT141</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>45688.88619232506</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>45688.88624818008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enhance analytics tracking in Studying functionality; persist session duration and update end time for same-day courses
</commit_message>
<xml_diff>
--- a/store/analytics.xlsx
+++ b/store/analytics.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,10 +485,298 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>45688.88619232506</v>
+        <v>45688.88619232639</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>45688.88624818008</v>
+        <v>45688.88624818287</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>MAT111</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>45688.8971716551</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>45688.89718125</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>MAT111</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>45688.89738734953</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>45688.897398125</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>MAT111</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>70</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>45688.89738734953</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>45688.89943899305</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>MAT111</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>35</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>45688.89926336805</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>45688.90001787037</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>MAT111</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>180</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>45688.89992260416</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>45688.93094452546</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>MAT111</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>45688.93066046296</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>45688.94555541666</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>MAT111</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>45688.94548275463</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>45688.94555541666</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>MAT141</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>45688.94568693287</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>45688.94571783565</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>MAT141</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>45688.94568693287</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>45688.94579412037</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>MAT141</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>45688.94576165509</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>45688.94579412037</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>MAT111</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>-4</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>45688.94782407407</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>45688.94783728009</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>MAT111</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>45688.94782407407</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>45688.94946922454</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>MAT111</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>4</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>45688.94940972222</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>45688.94946922454</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>MAT141</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>3</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>45688.94949074074</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>45688.94957386574</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>MAT141</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>6</v>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>45688.94949074074</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>45688.94986707176</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>MAT141</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>19</v>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>45688.94960648148</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>45688.94986707176</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>MAT111</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>5</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>45688.95012731481</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>45688.95017834491</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>MAT111</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>7</v>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>45688.95012731481</v>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>45688.95017834548</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor analytics tracking in Studying functionality; improve same-day course handling and update session duration logic
</commit_message>
<xml_diff>
--- a/store/analytics.xlsx
+++ b/store/analytics.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,33 +462,33 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MAT141</t>
+          <t>CSC103</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>45688.88619232639</v>
+        <v>45689.57058857639</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>45688.88624818287</v>
+        <v>45689.57061342592</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MAT141</t>
+          <t>CSC103</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>45688.88619232639</v>
+        <v>45689.57058857639</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>45688.88624818287</v>
+        <v>45689.57890046296</v>
       </c>
     </row>
     <row r="4">
@@ -498,285 +498,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>45688.8971716551</v>
+        <v>45689.58032532407</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>45688.89718125</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>MAT111</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>45688.89738734953</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>45688.897398125</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>MAT111</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>70</v>
-      </c>
-      <c r="C6" s="2" t="n">
-        <v>45688.89738734953</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>45688.89943899305</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>MAT111</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>35</v>
-      </c>
-      <c r="C7" s="2" t="n">
-        <v>45688.89926336805</v>
-      </c>
-      <c r="D7" s="2" t="n">
-        <v>45688.90001787037</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>MAT111</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>180</v>
-      </c>
-      <c r="C8" s="2" t="n">
-        <v>45688.89992260416</v>
-      </c>
-      <c r="D8" s="2" t="n">
-        <v>45688.93094452546</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>MAT111</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>24</v>
-      </c>
-      <c r="C9" s="2" t="n">
-        <v>45688.93066046296</v>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>45688.94555541666</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>MAT111</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>6</v>
-      </c>
-      <c r="C10" s="2" t="n">
-        <v>45688.94548275463</v>
-      </c>
-      <c r="D10" s="2" t="n">
-        <v>45688.94555541666</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>MAT141</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" s="2" t="n">
-        <v>45688.94568693287</v>
-      </c>
-      <c r="D11" s="2" t="n">
-        <v>45688.94571783565</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>MAT141</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>2</v>
-      </c>
-      <c r="C12" s="2" t="n">
-        <v>45688.94568693287</v>
-      </c>
-      <c r="D12" s="2" t="n">
-        <v>45688.94579412037</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>MAT141</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>2</v>
-      </c>
-      <c r="C13" s="2" t="n">
-        <v>45688.94576165509</v>
-      </c>
-      <c r="D13" s="2" t="n">
-        <v>45688.94579412037</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>MAT111</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>-4</v>
-      </c>
-      <c r="C14" s="2" t="n">
-        <v>45688.94782407407</v>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>45688.94783728009</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>MAT111</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" s="2" t="n">
-        <v>45688.94782407407</v>
-      </c>
-      <c r="D15" s="2" t="n">
-        <v>45688.94946922454</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>MAT111</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>4</v>
-      </c>
-      <c r="C16" s="2" t="n">
-        <v>45688.94940972222</v>
-      </c>
-      <c r="D16" s="2" t="n">
-        <v>45688.94946922454</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>MAT141</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>3</v>
-      </c>
-      <c r="C17" s="2" t="n">
-        <v>45688.94949074074</v>
-      </c>
-      <c r="D17" s="2" t="n">
-        <v>45688.94957386574</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>MAT141</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>6</v>
-      </c>
-      <c r="C18" s="2" t="n">
-        <v>45688.94949074074</v>
-      </c>
-      <c r="D18" s="2" t="n">
-        <v>45688.94986707176</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>MAT141</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>19</v>
-      </c>
-      <c r="C19" s="2" t="n">
-        <v>45688.94960648148</v>
-      </c>
-      <c r="D19" s="2" t="n">
-        <v>45688.94986707176</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>MAT111</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>5</v>
-      </c>
-      <c r="C20" s="2" t="n">
-        <v>45688.95012731481</v>
-      </c>
-      <c r="D20" s="2" t="n">
-        <v>45688.95017834491</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>MAT111</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>7</v>
-      </c>
-      <c r="C21" s="2" t="n">
-        <v>45688.95012731481</v>
-      </c>
-      <c r="D21" s="2" t="n">
-        <v>45688.95017834548</v>
+        <v>45689.58048611111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Analysis page for weekly study analytics; integrate data visualization and navigation
</commit_message>
<xml_diff>
--- a/store/analytics.xlsx
+++ b/store/analytics.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,13 +482,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>45689.57058857639</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>45689.57890046296</v>
+        <v>45689.68715491898</v>
       </c>
     </row>
     <row r="4">
@@ -498,13 +498,29 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>45689.58032532407</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>45689.58048611111</v>
+        <v>45689.68215277778</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>MAT141</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>45689.68708708333</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>45689.68714495492</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement reload functionality for UI refresh across multiple pages; enhance data handling in MainPage, Analysis, and Timetable
</commit_message>
<xml_diff>
--- a/store/analytics.xlsx
+++ b/store/analytics.xlsx
@@ -482,13 +482,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>45689.57058857639</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>45689.68715491898</v>
+        <v>45689.69406865988</v>
       </c>
     </row>
     <row r="4">
@@ -520,7 +520,7 @@
         <v>45689.68708708333</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>45689.68714495492</v>
+        <v>45689.68714495371</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix closure issue in MainPage study buttons; create command factory for button actions
</commit_message>
<xml_diff>
--- a/store/analytics.xlsx
+++ b/store/analytics.xlsx
@@ -482,13 +482,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>45689.57058857639</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>45689.69406865988</v>
+        <v>45689.6969383912</v>
       </c>
     </row>
     <row r="4">
@@ -498,13 +498,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>45689.58032532407</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>45689.68215277778</v>
+        <v>45689.69669267517</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Enhance profile submission validation; update timetable structure and reload functionality across pages
</commit_message>
<xml_diff>
--- a/store/analytics.xlsx
+++ b/store/analytics.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,7 +504,7 @@
         <v>45689.58032532407</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>45689.69669267517</v>
+        <v>45689.69669267361</v>
       </c>
     </row>
     <row r="5">
@@ -520,7 +520,55 @@
         <v>45689.68708708333</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>45689.68714495371</v>
+        <v>45689.74915857639</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>CUSTOM</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>45689.73709944444</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>45689.74339052083</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>MAT151</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>45689.73989837963</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>45689.73992152778</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>MILLONIARA</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>45689.75070482639</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>45689.75072797792</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor MainPage to Dashboard; update navigation and reload functionality across Studying and Timetable pages
</commit_message>
<xml_diff>
--- a/store/analytics.xlsx
+++ b/store/analytics.xlsx
@@ -520,7 +520,7 @@
         <v>45689.68708708333</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>45689.74915857639</v>
+        <v>45689.76323081694</v>
       </c>
     </row>
     <row r="6">
@@ -562,13 +562,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>45689.75070482639</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>45689.75072797792</v>
+        <v>45689.76050114584</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor navigation to use Dashboard instead of MainPage; update related commands and reload functionality in UploadMaterials and App
</commit_message>
<xml_diff>
--- a/store/analytics.xlsx
+++ b/store/analytics.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -520,7 +520,7 @@
         <v>45689.68708708333</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>45689.76323081694</v>
+        <v>45689.76860903935</v>
       </c>
     </row>
     <row r="6">
@@ -562,13 +562,29 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>45689.75070482639</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>45689.76050114584</v>
+        <v>45689.76876608796</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>aaaaaa</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>45689.76918370945</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>45689.76918370945</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor store_courses method to conditionally navigate to Dashboard; update timetable.json to clear Thursday courses and clean up unnecessary entries
</commit_message>
<xml_diff>
--- a/store/analytics.xlsx
+++ b/store/analytics.xlsx
@@ -520,7 +520,7 @@
         <v>45689.68708708333</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>45689.76860903935</v>
+        <v>45689.77322040848</v>
       </c>
     </row>
     <row r="6">
@@ -581,10 +581,10 @@
         <v>0</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>45689.76918370945</v>
+        <v>45689.76918370371</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>45689.76918370945</v>
+        <v>45689.76918370371</v>
       </c>
     </row>
   </sheetData>

</xml_diff>